<commit_message>
Day 5 Completed | DA 22
</commit_message>
<xml_diff>
--- a/batches/22/day_05/day_05.xlsx
+++ b/batches/22/day_05/day_05.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11202"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11203"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shira/Documents/work/acciojob/modules/sql/batches/22/day_05/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3BC43CE-56D0-134A-9D73-73CF3EC3CE29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3231055B-707C-7747-AD3E-98D1A7F375EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="21600" activeTab="3" xr2:uid="{C1255886-1A36-7049-922C-94975393B49A}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="21600" activeTab="4" xr2:uid="{C1255886-1A36-7049-922C-94975393B49A}"/>
   </bookViews>
   <sheets>
     <sheet name="Recap" sheetId="1" r:id="rId1"/>
     <sheet name="Agenda" sheetId="2" r:id="rId2"/>
     <sheet name="Constraints" sheetId="3" r:id="rId3"/>
     <sheet name="Filtering" sheetId="4" r:id="rId4"/>
+    <sheet name="advance_filtering" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="423" uniqueCount="232">
   <si>
     <t>🔄 WHAT WE'VE LEARNED SO FAR:</t>
   </si>
@@ -378,19 +379,390 @@
   </si>
   <si>
     <t>Filtering</t>
+  </si>
+  <si>
+    <t>full_name</t>
+  </si>
+  <si>
+    <t>gender</t>
+  </si>
+  <si>
+    <t>age</t>
+  </si>
+  <si>
+    <t>city</t>
+  </si>
+  <si>
+    <t>state</t>
+  </si>
+  <si>
+    <t>join_date</t>
+  </si>
+  <si>
+    <t>region_name</t>
+  </si>
+  <si>
+    <t>Pallavi Vyas</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>Chandigarh</t>
+  </si>
+  <si>
+    <t>Punjab</t>
+  </si>
+  <si>
+    <t>East</t>
+  </si>
+  <si>
+    <t>Deepti Kashyap</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>Gaya</t>
+  </si>
+  <si>
+    <t>Bihar</t>
+  </si>
+  <si>
+    <t>West</t>
+  </si>
+  <si>
+    <t>Kritika Siddiqui</t>
+  </si>
+  <si>
+    <t>Cuttack</t>
+  </si>
+  <si>
+    <t>Odisha</t>
+  </si>
+  <si>
+    <t>North</t>
+  </si>
+  <si>
+    <t>Sagar Kashyap</t>
+  </si>
+  <si>
+    <t>Muzaffarpur</t>
+  </si>
+  <si>
+    <t>Central</t>
+  </si>
+  <si>
+    <t>Manav Shah</t>
+  </si>
+  <si>
+    <t>Nikhil Chatterjee</t>
+  </si>
+  <si>
+    <t>Leh</t>
+  </si>
+  <si>
+    <t>Ladakh</t>
+  </si>
+  <si>
+    <t>Sonali Rai</t>
+  </si>
+  <si>
+    <t>Gwalior</t>
+  </si>
+  <si>
+    <t>Madhya Pradesh</t>
+  </si>
+  <si>
+    <t>Jaspreet Mishra</t>
+  </si>
+  <si>
+    <t>South</t>
+  </si>
+  <si>
+    <t>Yuvraj Tripathi</t>
+  </si>
+  <si>
+    <t>Meerut</t>
+  </si>
+  <si>
+    <t>Uttar Pradesh</t>
+  </si>
+  <si>
+    <t>Bhoomi Bhandari</t>
+  </si>
+  <si>
+    <t>Vinay Mehta</t>
+  </si>
+  <si>
+    <t>Bhubaneswar</t>
+  </si>
+  <si>
+    <t>Manoj Basu</t>
+  </si>
+  <si>
+    <t>Vadodara</t>
+  </si>
+  <si>
+    <t>Gujarat</t>
+  </si>
+  <si>
+    <t>Deepti Bhatia</t>
+  </si>
+  <si>
+    <t>Naman Dev</t>
+  </si>
+  <si>
+    <t>Patiala</t>
+  </si>
+  <si>
+    <t>Dev Bansal</t>
+  </si>
+  <si>
+    <t>Rourkela</t>
+  </si>
+  <si>
+    <t>Parth Mahajan</t>
+  </si>
+  <si>
+    <t>Karimnagar</t>
+  </si>
+  <si>
+    <t>Telangana</t>
+  </si>
+  <si>
+    <t>Trisha Naidu</t>
+  </si>
+  <si>
+    <t>Aizawl</t>
+  </si>
+  <si>
+    <t>Mizoram</t>
+  </si>
+  <si>
+    <t>Naman Prasad</t>
+  </si>
+  <si>
+    <t>Rajkot</t>
+  </si>
+  <si>
+    <t>Preeti Tandon</t>
+  </si>
+  <si>
+    <t>Shimla</t>
+  </si>
+  <si>
+    <t>Himachal Pradesh</t>
+  </si>
+  <si>
+    <t>Pankaj Chopra</t>
+  </si>
+  <si>
+    <t>Noida</t>
+  </si>
+  <si>
+    <t>Nisha Goswami</t>
+  </si>
+  <si>
+    <t>Udaipur</t>
+  </si>
+  <si>
+    <t>Rajasthan</t>
+  </si>
+  <si>
+    <t>Gauri Reddy</t>
+  </si>
+  <si>
+    <t>Ludhiana</t>
+  </si>
+  <si>
+    <t>Ira Malhotra</t>
+  </si>
+  <si>
+    <t>Agra</t>
+  </si>
+  <si>
+    <t>Jayant Verma</t>
+  </si>
+  <si>
+    <t>Thane</t>
+  </si>
+  <si>
+    <t>Maharashtra</t>
+  </si>
+  <si>
+    <t>Tanisha Kaul</t>
+  </si>
+  <si>
+    <t>Amrita Bhosale</t>
+  </si>
+  <si>
+    <t>Aarav Nath</t>
+  </si>
+  <si>
+    <t>Amritsar</t>
+  </si>
+  <si>
+    <t>Gautam Dev</t>
+  </si>
+  <si>
+    <t>Rahul Modi</t>
+  </si>
+  <si>
+    <t>Howrah</t>
+  </si>
+  <si>
+    <t>West Bengal</t>
+  </si>
+  <si>
+    <t>Manisha Vyas</t>
+  </si>
+  <si>
+    <t>Ira Saha</t>
+  </si>
+  <si>
+    <t>Priya Tandon</t>
+  </si>
+  <si>
+    <t>Panaji</t>
+  </si>
+  <si>
+    <t>Goa</t>
+  </si>
+  <si>
+    <t>Uma Rastogi</t>
+  </si>
+  <si>
+    <t>Ishan Fernandes</t>
+  </si>
+  <si>
+    <t>Salem</t>
+  </si>
+  <si>
+    <t>Tamil Nadu</t>
+  </si>
+  <si>
+    <t>Sana Mukherjee</t>
+  </si>
+  <si>
+    <t>Sanjay Joshi</t>
+  </si>
+  <si>
+    <t>Trichy</t>
+  </si>
+  <si>
+    <t>Tanmay Deshmukh</t>
+  </si>
+  <si>
+    <t>Aparna Kaul</t>
+  </si>
+  <si>
+    <t>Surat</t>
+  </si>
+  <si>
+    <t>Gautam Mohanty</t>
+  </si>
+  <si>
+    <t>Prateek Pillai</t>
+  </si>
+  <si>
+    <t>Kolkata</t>
+  </si>
+  <si>
+    <t>Anjali Kaul</t>
+  </si>
+  <si>
+    <t>Bhopal</t>
+  </si>
+  <si>
+    <t>Suhana Dasgupta</t>
+  </si>
+  <si>
+    <t>Sana Joshi</t>
+  </si>
+  <si>
+    <t>Omkar Patel</t>
+  </si>
+  <si>
+    <t>Pooja Duggal</t>
+  </si>
+  <si>
+    <t>Puri</t>
+  </si>
+  <si>
+    <t>Meera Bose</t>
+  </si>
+  <si>
+    <t>Udupi</t>
+  </si>
+  <si>
+    <t>Karnataka</t>
+  </si>
+  <si>
+    <t>Manoj Kaur</t>
+  </si>
+  <si>
+    <t>New Delhi</t>
+  </si>
+  <si>
+    <t>Delhi</t>
+  </si>
+  <si>
+    <t>Pankaj Mohanty</t>
+  </si>
+  <si>
+    <t>Prakash Bhandari</t>
+  </si>
+  <si>
+    <t>Dhanbad</t>
+  </si>
+  <si>
+    <t>Jharkhand</t>
+  </si>
+  <si>
+    <t>Madhav Gill</t>
+  </si>
+  <si>
+    <t>State</t>
+  </si>
+  <si>
+    <t>Manav</t>
+  </si>
+  <si>
+    <t>Starts with S</t>
+  </si>
+  <si>
+    <t>"S*"</t>
+  </si>
+  <si>
+    <t>"*S"</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="169" formatCode="dd/mm/yyyy;@"/>
+  </numFmts>
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Helvetica Neue"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Helvetica Neue"/>
     </font>
   </fonts>
   <fills count="4">
@@ -462,13 +834,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="169" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="169" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -696,8 +1073,8 @@
       <xdr:row>66</xdr:row>
       <xdr:rowOff>156177</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId7">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="5" name="Ink 4">
@@ -716,7 +1093,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="5" name="Ink 4">
@@ -761,8 +1138,8 @@
       <xdr:row>66</xdr:row>
       <xdr:rowOff>200817</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId9">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="6" name="Ink 5">
@@ -781,7 +1158,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="6" name="Ink 5">
@@ -1275,8 +1652,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A7498CA-705E-BC47-BC1B-57CDC8C7DF82}">
   <dimension ref="B2:B39"/>
   <sheetViews>
-    <sheetView topLeftCell="A27" zoomScale="266" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView topLeftCell="A25" zoomScale="266" workbookViewId="0">
+      <selection activeCell="B37" sqref="B37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1446,7 +1823,7 @@
   <dimension ref="B2:B31"/>
   <sheetViews>
     <sheetView topLeftCell="A13" zoomScale="226" workbookViewId="0">
-      <selection activeCell="F29" sqref="F29"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2112,8 +2489,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{381F2526-F31E-5247-AC85-802FB81EA46D}">
   <dimension ref="B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="398" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView zoomScale="398" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2129,4 +2506,1381 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC3A5933-2D74-C543-B348-D9965D831D5A}">
+  <dimension ref="B2:L52"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="272" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="6.1640625" customWidth="1"/>
+    <col min="2" max="2" width="7" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="4.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.1640625" style="8" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B2" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="H2" s="9" t="s">
+        <v>118</v>
+      </c>
+      <c r="I2" s="6" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="3" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B3" s="6">
+        <v>23</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>178</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="E3" s="7">
+        <v>20</v>
+      </c>
+      <c r="F3" s="7" t="s">
+        <v>179</v>
+      </c>
+      <c r="G3" s="7" t="s">
+        <v>148</v>
+      </c>
+      <c r="H3" s="10">
+        <v>45308</v>
+      </c>
+      <c r="I3" s="7" t="s">
+        <v>133</v>
+      </c>
+      <c r="K3" s="7" t="s">
+        <v>227</v>
+      </c>
+      <c r="L3" s="7" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="4" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B4" s="6">
+        <v>17</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>163</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="E4" s="7">
+        <v>21</v>
+      </c>
+      <c r="F4" s="7" t="s">
+        <v>164</v>
+      </c>
+      <c r="G4" s="7" t="s">
+        <v>165</v>
+      </c>
+      <c r="H4" s="10">
+        <v>44726</v>
+      </c>
+      <c r="I4" s="7" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="5" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B5" s="6">
+        <v>27</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>185</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="E5" s="7">
+        <v>41</v>
+      </c>
+      <c r="F5" s="7" t="s">
+        <v>186</v>
+      </c>
+      <c r="G5" s="7" t="s">
+        <v>123</v>
+      </c>
+      <c r="H5" s="10">
+        <v>44610</v>
+      </c>
+      <c r="I5" s="7" t="s">
+        <v>124</v>
+      </c>
+      <c r="K5" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="L5" s="7" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="6" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B6" s="6">
+        <v>41</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>209</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>126</v>
+      </c>
+      <c r="E6" s="7">
+        <v>60</v>
+      </c>
+      <c r="F6" s="7" t="s">
+        <v>210</v>
+      </c>
+      <c r="G6" s="7" t="s">
+        <v>143</v>
+      </c>
+      <c r="H6" s="10">
+        <v>44610</v>
+      </c>
+      <c r="I6" s="7" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="7" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B7" s="6">
+        <v>25</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>183</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>126</v>
+      </c>
+      <c r="E7" s="7">
+        <v>32</v>
+      </c>
+      <c r="F7" s="7" t="s">
+        <v>151</v>
+      </c>
+      <c r="G7" s="7" t="s">
+        <v>132</v>
+      </c>
+      <c r="H7" s="10">
+        <v>44610</v>
+      </c>
+      <c r="I7" s="7" t="s">
+        <v>145</v>
+      </c>
+      <c r="K7" s="7" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="8" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B8" s="6">
+        <v>11</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>150</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="E8" s="7">
+        <v>33</v>
+      </c>
+      <c r="F8" s="7" t="s">
+        <v>151</v>
+      </c>
+      <c r="G8" s="7" t="s">
+        <v>132</v>
+      </c>
+      <c r="H8" s="10">
+        <v>44610</v>
+      </c>
+      <c r="I8" s="7" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="9" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B9" s="6">
+        <v>31</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>192</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="E9" s="7">
+        <v>24</v>
+      </c>
+      <c r="F9" s="7" t="s">
+        <v>122</v>
+      </c>
+      <c r="G9" s="7" t="s">
+        <v>123</v>
+      </c>
+      <c r="H9" s="10">
+        <v>45010</v>
+      </c>
+      <c r="I9" s="7" t="s">
+        <v>145</v>
+      </c>
+      <c r="K9" s="7" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="10" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B10" s="6">
+        <v>1</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="D10" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="E10" s="7">
+        <v>28</v>
+      </c>
+      <c r="F10" s="7" t="s">
+        <v>122</v>
+      </c>
+      <c r="G10" s="7" t="s">
+        <v>123</v>
+      </c>
+      <c r="H10" s="10">
+        <v>45258</v>
+      </c>
+      <c r="I10" s="7" t="s">
+        <v>124</v>
+      </c>
+      <c r="K10" s="7" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="11" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B11" s="6">
+        <v>13</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>126</v>
+      </c>
+      <c r="E11" s="7">
+        <v>40</v>
+      </c>
+      <c r="F11" s="7" t="s">
+        <v>122</v>
+      </c>
+      <c r="G11" s="7" t="s">
+        <v>123</v>
+      </c>
+      <c r="H11" s="10">
+        <v>45403</v>
+      </c>
+      <c r="I11" s="7" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="12" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B12" s="6">
+        <v>5</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>137</v>
+      </c>
+      <c r="D12" s="7" t="s">
+        <v>126</v>
+      </c>
+      <c r="E12" s="7">
+        <v>21</v>
+      </c>
+      <c r="F12" s="7" t="s">
+        <v>131</v>
+      </c>
+      <c r="G12" s="7" t="s">
+        <v>132</v>
+      </c>
+      <c r="H12" s="10">
+        <v>44610</v>
+      </c>
+      <c r="I12" s="7" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="13" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B13" s="6">
+        <v>3</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="D13" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="E13" s="7">
+        <v>20</v>
+      </c>
+      <c r="F13" s="7" t="s">
+        <v>131</v>
+      </c>
+      <c r="G13" s="7" t="s">
+        <v>132</v>
+      </c>
+      <c r="H13" s="10">
+        <v>45154</v>
+      </c>
+      <c r="I13" s="7" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="14" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B14" s="6">
+        <v>49</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>223</v>
+      </c>
+      <c r="D14" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="E14" s="7">
+        <v>25</v>
+      </c>
+      <c r="F14" s="7" t="s">
+        <v>224</v>
+      </c>
+      <c r="G14" s="7" t="s">
+        <v>225</v>
+      </c>
+      <c r="H14" s="10">
+        <v>45024</v>
+      </c>
+      <c r="I14" s="7" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="15" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B15" s="6">
+        <v>26</v>
+      </c>
+      <c r="C15" s="7" t="s">
+        <v>184</v>
+      </c>
+      <c r="D15" s="7" t="s">
+        <v>126</v>
+      </c>
+      <c r="E15" s="7">
+        <v>29</v>
+      </c>
+      <c r="F15" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="G15" s="7" t="s">
+        <v>128</v>
+      </c>
+      <c r="H15" s="10">
+        <v>44610</v>
+      </c>
+      <c r="I15" s="7" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="16" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B16" s="6">
+        <v>2</v>
+      </c>
+      <c r="C16" s="7" t="s">
+        <v>125</v>
+      </c>
+      <c r="D16" s="7" t="s">
+        <v>126</v>
+      </c>
+      <c r="E16" s="7">
+        <v>56</v>
+      </c>
+      <c r="F16" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="G16" s="7" t="s">
+        <v>128</v>
+      </c>
+      <c r="H16" s="10">
+        <v>44610</v>
+      </c>
+      <c r="I16" s="7" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="17" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B17" s="6">
+        <v>8</v>
+      </c>
+      <c r="C17" s="7" t="s">
+        <v>144</v>
+      </c>
+      <c r="D17" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="E17" s="7">
+        <v>64</v>
+      </c>
+      <c r="F17" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="G17" s="7" t="s">
+        <v>128</v>
+      </c>
+      <c r="H17" s="10">
+        <v>45587</v>
+      </c>
+      <c r="I17" s="7" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="18" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B18" s="6">
+        <v>28</v>
+      </c>
+      <c r="C18" s="7" t="s">
+        <v>187</v>
+      </c>
+      <c r="D18" s="7" t="s">
+        <v>126</v>
+      </c>
+      <c r="E18" s="7">
+        <v>60</v>
+      </c>
+      <c r="F18" s="7" t="s">
+        <v>142</v>
+      </c>
+      <c r="G18" s="7" t="s">
+        <v>143</v>
+      </c>
+      <c r="H18" s="10">
+        <v>44918</v>
+      </c>
+      <c r="I18" s="7" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="19" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B19" s="6">
+        <v>37</v>
+      </c>
+      <c r="C19" s="7" t="s">
+        <v>203</v>
+      </c>
+      <c r="D19" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="E19" s="7">
+        <v>34</v>
+      </c>
+      <c r="F19" s="7" t="s">
+        <v>142</v>
+      </c>
+      <c r="G19" s="7" t="s">
+        <v>143</v>
+      </c>
+      <c r="H19" s="10">
+        <v>45232</v>
+      </c>
+      <c r="I19" s="7" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="20" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B20" s="6">
+        <v>7</v>
+      </c>
+      <c r="C20" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="D20" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="E20" s="7">
+        <v>42</v>
+      </c>
+      <c r="F20" s="7" t="s">
+        <v>142</v>
+      </c>
+      <c r="G20" s="7" t="s">
+        <v>143</v>
+      </c>
+      <c r="H20" s="10">
+        <v>45520</v>
+      </c>
+      <c r="I20" s="7" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="21" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B21" s="6">
+        <v>39</v>
+      </c>
+      <c r="C21" s="7" t="s">
+        <v>206</v>
+      </c>
+      <c r="D21" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="E21" s="7">
+        <v>54</v>
+      </c>
+      <c r="F21" s="7" t="s">
+        <v>189</v>
+      </c>
+      <c r="G21" s="7" t="s">
+        <v>190</v>
+      </c>
+      <c r="H21" s="10">
+        <v>45514</v>
+      </c>
+      <c r="I21" s="7" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="22" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B22" s="6">
+        <v>29</v>
+      </c>
+      <c r="C22" s="7" t="s">
+        <v>188</v>
+      </c>
+      <c r="D22" s="7" t="s">
+        <v>126</v>
+      </c>
+      <c r="E22" s="7">
+        <v>46</v>
+      </c>
+      <c r="F22" s="7" t="s">
+        <v>189</v>
+      </c>
+      <c r="G22" s="7" t="s">
+        <v>190</v>
+      </c>
+      <c r="H22" s="10">
+        <v>45608</v>
+      </c>
+      <c r="I22" s="7" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="23" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B23" s="6">
+        <v>44</v>
+      </c>
+      <c r="C23" s="7" t="s">
+        <v>213</v>
+      </c>
+      <c r="D23" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="E23" s="7">
+        <v>51</v>
+      </c>
+      <c r="F23" s="7" t="s">
+        <v>161</v>
+      </c>
+      <c r="G23" s="7" t="s">
+        <v>162</v>
+      </c>
+      <c r="H23" s="10">
+        <v>44737</v>
+      </c>
+      <c r="I23" s="7" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="24" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B24" s="6">
+        <v>16</v>
+      </c>
+      <c r="C24" s="7" t="s">
+        <v>160</v>
+      </c>
+      <c r="D24" s="7" t="s">
+        <v>126</v>
+      </c>
+      <c r="E24" s="7">
+        <v>27</v>
+      </c>
+      <c r="F24" s="7" t="s">
+        <v>161</v>
+      </c>
+      <c r="G24" s="7" t="s">
+        <v>162</v>
+      </c>
+      <c r="H24" s="10">
+        <v>45169</v>
+      </c>
+      <c r="I24" s="7" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="25" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B25" s="6">
+        <v>40</v>
+      </c>
+      <c r="C25" s="7" t="s">
+        <v>207</v>
+      </c>
+      <c r="D25" s="7" t="s">
+        <v>126</v>
+      </c>
+      <c r="E25" s="7">
+        <v>43</v>
+      </c>
+      <c r="F25" s="7" t="s">
+        <v>208</v>
+      </c>
+      <c r="G25" s="7" t="s">
+        <v>190</v>
+      </c>
+      <c r="H25" s="10">
+        <v>44610</v>
+      </c>
+      <c r="I25" s="7" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="26" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B26" s="6">
+        <v>10</v>
+      </c>
+      <c r="C26" s="7" t="s">
+        <v>149</v>
+      </c>
+      <c r="D26" s="7" t="s">
+        <v>126</v>
+      </c>
+      <c r="E26" s="7">
+        <v>22</v>
+      </c>
+      <c r="F26" s="7" t="s">
+        <v>139</v>
+      </c>
+      <c r="G26" s="7" t="s">
+        <v>140</v>
+      </c>
+      <c r="H26" s="10">
+        <v>44819</v>
+      </c>
+      <c r="I26" s="7" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="27" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B27" s="6">
+        <v>6</v>
+      </c>
+      <c r="C27" s="7" t="s">
+        <v>138</v>
+      </c>
+      <c r="D27" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="E27" s="7">
+        <v>65</v>
+      </c>
+      <c r="F27" s="7" t="s">
+        <v>139</v>
+      </c>
+      <c r="G27" s="7" t="s">
+        <v>140</v>
+      </c>
+      <c r="H27" s="10">
+        <v>45100</v>
+      </c>
+      <c r="I27" s="7" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="28" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B28" s="6">
+        <v>42</v>
+      </c>
+      <c r="C28" s="7" t="s">
+        <v>211</v>
+      </c>
+      <c r="D28" s="7" t="s">
+        <v>126</v>
+      </c>
+      <c r="E28" s="7">
+        <v>57</v>
+      </c>
+      <c r="F28" s="7" t="s">
+        <v>139</v>
+      </c>
+      <c r="G28" s="7" t="s">
+        <v>140</v>
+      </c>
+      <c r="H28" s="10">
+        <v>45552</v>
+      </c>
+      <c r="I28" s="7" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="29" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B29" s="6">
+        <v>33</v>
+      </c>
+      <c r="C29" s="7" t="s">
+        <v>196</v>
+      </c>
+      <c r="D29" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="E29" s="7">
+        <v>35</v>
+      </c>
+      <c r="F29" s="7" t="s">
+        <v>177</v>
+      </c>
+      <c r="G29" s="7" t="s">
+        <v>123</v>
+      </c>
+      <c r="H29" s="10">
+        <v>44610</v>
+      </c>
+      <c r="I29" s="7" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="30" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B30" s="6">
+        <v>22</v>
+      </c>
+      <c r="C30" s="7" t="s">
+        <v>176</v>
+      </c>
+      <c r="D30" s="7" t="s">
+        <v>126</v>
+      </c>
+      <c r="E30" s="7">
+        <v>28</v>
+      </c>
+      <c r="F30" s="7" t="s">
+        <v>177</v>
+      </c>
+      <c r="G30" s="7" t="s">
+        <v>123</v>
+      </c>
+      <c r="H30" s="10">
+        <v>45437</v>
+      </c>
+      <c r="I30" s="7" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="31" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B31" s="6">
+        <v>43</v>
+      </c>
+      <c r="C31" s="7" t="s">
+        <v>212</v>
+      </c>
+      <c r="D31" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="E31" s="7">
+        <v>49</v>
+      </c>
+      <c r="F31" s="7" t="s">
+        <v>147</v>
+      </c>
+      <c r="G31" s="7" t="s">
+        <v>148</v>
+      </c>
+      <c r="H31" s="10">
+        <v>44934</v>
+      </c>
+      <c r="I31" s="7" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="32" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B32" s="6">
+        <v>9</v>
+      </c>
+      <c r="C32" s="7" t="s">
+        <v>146</v>
+      </c>
+      <c r="D32" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="E32" s="7">
+        <v>56</v>
+      </c>
+      <c r="F32" s="7" t="s">
+        <v>147</v>
+      </c>
+      <c r="G32" s="7" t="s">
+        <v>148</v>
+      </c>
+      <c r="H32" s="10">
+        <v>45562</v>
+      </c>
+      <c r="I32" s="7" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="33" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B33" s="6">
+        <v>4</v>
+      </c>
+      <c r="C33" s="7" t="s">
+        <v>134</v>
+      </c>
+      <c r="D33" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="E33" s="7">
+        <v>60</v>
+      </c>
+      <c r="F33" s="7" t="s">
+        <v>135</v>
+      </c>
+      <c r="G33" s="7" t="s">
+        <v>128</v>
+      </c>
+      <c r="H33" s="10">
+        <v>44610</v>
+      </c>
+      <c r="I33" s="7" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="34" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B34" s="6">
+        <v>47</v>
+      </c>
+      <c r="C34" s="7" t="s">
+        <v>219</v>
+      </c>
+      <c r="D34" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="E34" s="7">
+        <v>37</v>
+      </c>
+      <c r="F34" s="7" t="s">
+        <v>220</v>
+      </c>
+      <c r="G34" s="7" t="s">
+        <v>221</v>
+      </c>
+      <c r="H34" s="10">
+        <v>45655</v>
+      </c>
+      <c r="I34" s="7" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="35" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B35" s="6">
+        <v>35</v>
+      </c>
+      <c r="C35" s="7" t="s">
+        <v>200</v>
+      </c>
+      <c r="D35" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="E35" s="7">
+        <v>40</v>
+      </c>
+      <c r="F35" s="7" t="s">
+        <v>172</v>
+      </c>
+      <c r="G35" s="7" t="s">
+        <v>148</v>
+      </c>
+      <c r="H35" s="10">
+        <v>45360</v>
+      </c>
+      <c r="I35" s="7" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="36" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B36" s="6">
+        <v>20</v>
+      </c>
+      <c r="C36" s="7" t="s">
+        <v>171</v>
+      </c>
+      <c r="D36" s="7" t="s">
+        <v>126</v>
+      </c>
+      <c r="E36" s="7">
+        <v>52</v>
+      </c>
+      <c r="F36" s="7" t="s">
+        <v>172</v>
+      </c>
+      <c r="G36" s="7" t="s">
+        <v>148</v>
+      </c>
+      <c r="H36" s="10">
+        <v>45645</v>
+      </c>
+      <c r="I36" s="7" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="37" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B37" s="6">
+        <v>32</v>
+      </c>
+      <c r="C37" s="7" t="s">
+        <v>193</v>
+      </c>
+      <c r="D37" s="7" t="s">
+        <v>126</v>
+      </c>
+      <c r="E37" s="7">
+        <v>57</v>
+      </c>
+      <c r="F37" s="7" t="s">
+        <v>194</v>
+      </c>
+      <c r="G37" s="7" t="s">
+        <v>195</v>
+      </c>
+      <c r="H37" s="10">
+        <v>45435</v>
+      </c>
+      <c r="I37" s="7" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="38" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B38" s="6">
+        <v>14</v>
+      </c>
+      <c r="C38" s="7" t="s">
+        <v>156</v>
+      </c>
+      <c r="D38" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="E38" s="7">
+        <v>52</v>
+      </c>
+      <c r="F38" s="7" t="s">
+        <v>157</v>
+      </c>
+      <c r="G38" s="7" t="s">
+        <v>123</v>
+      </c>
+      <c r="H38" s="10">
+        <v>44849</v>
+      </c>
+      <c r="I38" s="7" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="39" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B39" s="6">
+        <v>45</v>
+      </c>
+      <c r="C39" s="7" t="s">
+        <v>214</v>
+      </c>
+      <c r="D39" s="7" t="s">
+        <v>126</v>
+      </c>
+      <c r="E39" s="7">
+        <v>62</v>
+      </c>
+      <c r="F39" s="7" t="s">
+        <v>215</v>
+      </c>
+      <c r="G39" s="7" t="s">
+        <v>132</v>
+      </c>
+      <c r="H39" s="10">
+        <v>45189</v>
+      </c>
+      <c r="I39" s="7" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="40" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B40" s="6">
+        <v>18</v>
+      </c>
+      <c r="C40" s="7" t="s">
+        <v>166</v>
+      </c>
+      <c r="D40" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="E40" s="7">
+        <v>57</v>
+      </c>
+      <c r="F40" s="7" t="s">
+        <v>167</v>
+      </c>
+      <c r="G40" s="7" t="s">
+        <v>154</v>
+      </c>
+      <c r="H40" s="10">
+        <v>45420</v>
+      </c>
+      <c r="I40" s="7" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="41" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B41" s="6">
+        <v>15</v>
+      </c>
+      <c r="C41" s="7" t="s">
+        <v>158</v>
+      </c>
+      <c r="D41" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="E41" s="7">
+        <v>23</v>
+      </c>
+      <c r="F41" s="7" t="s">
+        <v>159</v>
+      </c>
+      <c r="G41" s="7" t="s">
+        <v>132</v>
+      </c>
+      <c r="H41" s="10">
+        <v>44902</v>
+      </c>
+      <c r="I41" s="7" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="42" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B42" s="6">
+        <v>50</v>
+      </c>
+      <c r="C42" s="7" t="s">
+        <v>226</v>
+      </c>
+      <c r="D42" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="E42" s="7">
+        <v>28</v>
+      </c>
+      <c r="F42" s="7" t="s">
+        <v>159</v>
+      </c>
+      <c r="G42" s="7" t="s">
+        <v>132</v>
+      </c>
+      <c r="H42" s="10">
+        <v>44917</v>
+      </c>
+      <c r="I42" s="7" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="43" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B43" s="6">
+        <v>34</v>
+      </c>
+      <c r="C43" s="7" t="s">
+        <v>197</v>
+      </c>
+      <c r="D43" s="7" t="s">
+        <v>126</v>
+      </c>
+      <c r="E43" s="7">
+        <v>62</v>
+      </c>
+      <c r="F43" s="7" t="s">
+        <v>198</v>
+      </c>
+      <c r="G43" s="7" t="s">
+        <v>199</v>
+      </c>
+      <c r="H43" s="10">
+        <v>45000</v>
+      </c>
+      <c r="I43" s="7" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="44" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B44" s="6">
+        <v>19</v>
+      </c>
+      <c r="C44" s="7" t="s">
+        <v>168</v>
+      </c>
+      <c r="D44" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="E44" s="7">
+        <v>18</v>
+      </c>
+      <c r="F44" s="7" t="s">
+        <v>169</v>
+      </c>
+      <c r="G44" s="7" t="s">
+        <v>170</v>
+      </c>
+      <c r="H44" s="10">
+        <v>44766</v>
+      </c>
+      <c r="I44" s="7" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="45" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B45" s="6">
+        <v>38</v>
+      </c>
+      <c r="C45" s="7" t="s">
+        <v>204</v>
+      </c>
+      <c r="D45" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="E45" s="7">
+        <v>59</v>
+      </c>
+      <c r="F45" s="7" t="s">
+        <v>205</v>
+      </c>
+      <c r="G45" s="7" t="s">
+        <v>154</v>
+      </c>
+      <c r="H45" s="10">
+        <v>44610</v>
+      </c>
+      <c r="I45" s="7" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="46" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B46" s="6">
+        <v>30</v>
+      </c>
+      <c r="C46" s="7" t="s">
+        <v>191</v>
+      </c>
+      <c r="D46" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="E46" s="7">
+        <v>27</v>
+      </c>
+      <c r="F46" s="7" t="s">
+        <v>181</v>
+      </c>
+      <c r="G46" s="7" t="s">
+        <v>182</v>
+      </c>
+      <c r="H46" s="10">
+        <v>44610</v>
+      </c>
+      <c r="I46" s="7" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="47" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B47" s="6">
+        <v>24</v>
+      </c>
+      <c r="C47" s="7" t="s">
+        <v>180</v>
+      </c>
+      <c r="D47" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="E47" s="7">
+        <v>44</v>
+      </c>
+      <c r="F47" s="7" t="s">
+        <v>181</v>
+      </c>
+      <c r="G47" s="7" t="s">
+        <v>182</v>
+      </c>
+      <c r="H47" s="10">
+        <v>44929</v>
+      </c>
+      <c r="I47" s="7" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="48" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B48" s="6">
+        <v>36</v>
+      </c>
+      <c r="C48" s="7" t="s">
+        <v>201</v>
+      </c>
+      <c r="D48" s="7" t="s">
+        <v>126</v>
+      </c>
+      <c r="E48" s="7">
+        <v>64</v>
+      </c>
+      <c r="F48" s="7" t="s">
+        <v>202</v>
+      </c>
+      <c r="G48" s="7" t="s">
+        <v>199</v>
+      </c>
+      <c r="H48" s="10">
+        <v>45519</v>
+      </c>
+      <c r="I48" s="7" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="49" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B49" s="6">
+        <v>48</v>
+      </c>
+      <c r="C49" s="7" t="s">
+        <v>222</v>
+      </c>
+      <c r="D49" s="7" t="s">
+        <v>126</v>
+      </c>
+      <c r="E49" s="7">
+        <v>46</v>
+      </c>
+      <c r="F49" s="7" t="s">
+        <v>174</v>
+      </c>
+      <c r="G49" s="7" t="s">
+        <v>175</v>
+      </c>
+      <c r="H49" s="10">
+        <v>44939</v>
+      </c>
+      <c r="I49" s="7" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="50" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B50" s="6">
+        <v>21</v>
+      </c>
+      <c r="C50" s="7" t="s">
+        <v>173</v>
+      </c>
+      <c r="D50" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="E50" s="7">
+        <v>63</v>
+      </c>
+      <c r="F50" s="7" t="s">
+        <v>174</v>
+      </c>
+      <c r="G50" s="7" t="s">
+        <v>175</v>
+      </c>
+      <c r="H50" s="10">
+        <v>44978</v>
+      </c>
+      <c r="I50" s="7" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="51" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B51" s="6">
+        <v>46</v>
+      </c>
+      <c r="C51" s="7" t="s">
+        <v>216</v>
+      </c>
+      <c r="D51" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="E51" s="7">
+        <v>38</v>
+      </c>
+      <c r="F51" s="7" t="s">
+        <v>217</v>
+      </c>
+      <c r="G51" s="7" t="s">
+        <v>218</v>
+      </c>
+      <c r="H51" s="10">
+        <v>44941</v>
+      </c>
+      <c r="I51" s="7" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="52" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B52" s="6">
+        <v>12</v>
+      </c>
+      <c r="C52" s="7" t="s">
+        <v>152</v>
+      </c>
+      <c r="D52" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="E52" s="7">
+        <v>39</v>
+      </c>
+      <c r="F52" s="7" t="s">
+        <v>153</v>
+      </c>
+      <c r="G52" s="7" t="s">
+        <v>154</v>
+      </c>
+      <c r="H52" s="10">
+        <v>45614</v>
+      </c>
+      <c r="I52" s="7" t="s">
+        <v>145</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B3:I52">
+    <sortCondition ref="F3:F52"/>
+    <sortCondition ref="H3:H52"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>